<commit_message>
fix: add solution to 18th, 9th tasks, and add variant.pdf
</commit_message>
<xml_diff>
--- a/EGE/online-olimpiada-ov-03-21/task_18.xlsx
+++ b/EGE/online-olimpiada-ov-03-21/task_18.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/htmlprogrammist/Python/ege/EGE/online-olimpiada-ov-03-21/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\ege\EGE\online-olimpiada-ov-03-21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264712A9-BB80-9149-A72A-AA50C40663E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71220EEB-74F2-453B-B658-621CA4C06EEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" xr2:uid="{6CF9F464-3206-461F-98B0-C1795E2DDBCA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6CF9F464-3206-461F-98B0-C1795E2DDBCA}"/>
   </bookViews>
   <sheets>
     <sheet name="18" sheetId="5" r:id="rId1"/>
@@ -25,9 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Старт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max = </t>
+  </si>
+  <si>
+    <t>842 ответ</t>
   </si>
 </sst>
 </file>
@@ -406,18 +412,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239A69A1-A0AE-4177-A121-45F2207588E7}">
-  <dimension ref="A1:U31"/>
+  <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="15" width="4.6640625" customWidth="1"/>
+    <col min="1" max="15" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>24</v>
       </c>
@@ -481,8 +487,24 @@
       <c r="U1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V1" s="2">
+        <f>W1+Q1</f>
+        <v>0</v>
+      </c>
+      <c r="W1" s="2">
+        <f>X1+R1</f>
+        <v>-4</v>
+      </c>
+      <c r="X1" s="2">
+        <f>T1+S1</f>
+        <v>-25</v>
+      </c>
+      <c r="Y1" s="2">
+        <f>T1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>8</v>
       </c>
@@ -540,8 +562,24 @@
       <c r="T2" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V2" s="2">
+        <f t="shared" ref="V2:W2" si="0">MAX(V1,W2,W1)+Q2</f>
+        <v>72</v>
+      </c>
+      <c r="W2" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="X2" s="2">
+        <f>MAX(X1,Y2,Y1)+S2</f>
+        <v>47</v>
+      </c>
+      <c r="Y2" s="2">
+        <f>Y1+T2</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>-10</v>
       </c>
@@ -599,8 +637,24 @@
       <c r="T3" s="2">
         <v>-5</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V3" s="2">
+        <f t="shared" ref="V3:V4" si="1">MAX(V2,W3,W2)+Q3</f>
+        <v>42</v>
+      </c>
+      <c r="W3" s="2">
+        <f t="shared" ref="W3:X4" si="2">MAX(W2,X3,X2)+R3</f>
+        <v>71</v>
+      </c>
+      <c r="X3" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="Y3" s="2">
+        <f>Y2+T3</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>58</v>
       </c>
@@ -658,8 +712,24 @@
       <c r="T4" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V4" s="2">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="W4" s="2">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="X4" s="2">
+        <f t="shared" ref="X4" si="3">MAX(X3,Y4,Y3)+S4</f>
+        <v>55</v>
+      </c>
+      <c r="Y4" s="2">
+        <f t="shared" ref="Y3:Y4" si="4">Y3+T4</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -705,8 +775,14 @@
       <c r="O5" s="1">
         <v>-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V5" t="s">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>-30</v>
       </c>
@@ -753,7 +829,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>-33</v>
       </c>
@@ -800,7 +876,7 @@
         <v>-17</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>14</v>
       </c>
@@ -847,7 +923,7 @@
         <v>-30</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44</v>
       </c>
@@ -894,7 +970,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>34</v>
       </c>
@@ -941,7 +1017,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>-31</v>
       </c>
@@ -988,7 +1064,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>53</v>
       </c>
@@ -1035,7 +1111,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>-28</v>
       </c>
@@ -1082,7 +1158,7 @@
         <v>-22</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>46</v>
       </c>
@@ -1129,7 +1205,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>56</v>
       </c>
@@ -1176,64 +1252,70 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="P16" s="5">
+        <f>MAX(N1,O2,O1)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <f t="shared" ref="A17:M17" si="0">B17+A1</f>
+        <f t="shared" ref="A17:L17" si="5">B17+A1</f>
         <v>323</v>
       </c>
       <c r="B17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>299</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>240</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>223</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>234</v>
       </c>
       <c r="F17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>233</v>
       </c>
       <c r="G17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>178</v>
       </c>
       <c r="I17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>148</v>
       </c>
       <c r="J17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>118</v>
       </c>
       <c r="K17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>97</v>
       </c>
       <c r="L17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>91</v>
       </c>
       <c r="M17" s="5">
-        <f t="shared" si="0"/>
+        <f>N17+M1</f>
         <v>108</v>
       </c>
       <c r="N17" s="5">
-        <f>O17+N1</f>
+        <f>O1+N1</f>
         <v>61</v>
       </c>
-      <c r="O17" s="3">
+      <c r="O17" s="2">
         <f>O1</f>
         <v>32</v>
       </c>
@@ -1241,11 +1323,11 @@
         <v>0</v>
       </c>
       <c r="Q17" s="2">
-        <f t="shared" ref="Q17:R17" si="1">R17+Q1</f>
+        <f t="shared" ref="Q17:R17" si="6">R17+Q1</f>
         <v>0</v>
       </c>
       <c r="R17" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>-4</v>
       </c>
       <c r="S17" s="2">
@@ -1260,29 +1342,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <f t="shared" ref="A18:M30" si="7">MAX(A17,B17,B18)+A2</f>
+        <v>331</v>
+      </c>
+      <c r="B18" s="5">
+        <f t="shared" si="7"/>
+        <v>288</v>
+      </c>
+      <c r="C18" s="5">
+        <f t="shared" si="7"/>
+        <v>206</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="7"/>
+        <v>232</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="7"/>
+        <v>270</v>
+      </c>
+      <c r="F18" s="5">
+        <f t="shared" si="7"/>
+        <v>253</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="7"/>
+        <v>263</v>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" si="7"/>
+        <v>234</v>
+      </c>
+      <c r="I18" s="5">
+        <f t="shared" si="7"/>
+        <v>109</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" si="7"/>
+        <v>118</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="7"/>
+        <v>102</v>
+      </c>
+      <c r="L18" s="5">
+        <f t="shared" si="7"/>
+        <v>89</v>
+      </c>
       <c r="M18" s="5">
-        <f>M17+M2</f>
+        <f t="shared" si="7"/>
         <v>107</v>
       </c>
       <c r="N18" s="5">
-        <f>O1+N2</f>
-        <v>8</v>
+        <f>MAX(N17,O17,O18)+N2</f>
+        <v>37</v>
       </c>
       <c r="O18" s="5">
-        <f>O17+O2</f>
+        <f>O1+O2</f>
         <v>7</v>
       </c>
       <c r="Q18" s="2"/>
@@ -1296,23 +1414,65 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <f t="shared" si="7"/>
+        <v>336</v>
+      </c>
+      <c r="B19" s="5">
+        <f t="shared" si="7"/>
+        <v>346</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" si="7"/>
+        <v>298</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="7"/>
+        <v>331</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="7"/>
+        <v>348</v>
+      </c>
+      <c r="F19" s="5">
+        <f t="shared" si="7"/>
+        <v>344</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="7"/>
+        <v>297</v>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" si="7"/>
+        <v>260</v>
+      </c>
+      <c r="I19" s="5">
+        <f t="shared" si="7"/>
+        <v>270</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" si="7"/>
+        <v>216</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" si="7"/>
+        <v>168</v>
+      </c>
+      <c r="L19" s="5">
+        <f t="shared" si="7"/>
+        <v>167</v>
+      </c>
+      <c r="M19" s="5">
+        <f t="shared" si="7"/>
+        <v>143</v>
+      </c>
+      <c r="N19" s="5">
+        <f t="shared" ref="N19:N30" si="8">MAX(N18,O18,O19)+N3</f>
+        <v>23</v>
+      </c>
       <c r="O19" s="5">
-        <f t="shared" ref="O19:O31" si="2">O18+O3</f>
+        <f>O18+O3</f>
         <v>12</v>
       </c>
       <c r="Q19" s="2"/>
@@ -1322,27 +1482,69 @@
       </c>
       <c r="S19" s="2"/>
       <c r="T19" s="2">
-        <f t="shared" ref="T19:T20" si="3">T18+T3</f>
+        <f t="shared" ref="T19:T20" si="9">T18+T3</f>
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <f t="shared" si="7"/>
+        <v>514</v>
+      </c>
+      <c r="B20" s="5">
+        <f t="shared" si="7"/>
+        <v>456</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" si="7"/>
+        <v>412</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" si="7"/>
+        <v>383</v>
+      </c>
+      <c r="E20" s="5">
+        <f t="shared" si="7"/>
+        <v>421</v>
+      </c>
+      <c r="F20" s="5">
+        <f t="shared" si="7"/>
+        <v>434</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="7"/>
+        <v>378</v>
+      </c>
+      <c r="H20" s="5">
+        <f t="shared" si="7"/>
+        <v>329</v>
+      </c>
+      <c r="I20" s="5">
+        <f t="shared" si="7"/>
+        <v>247</v>
+      </c>
+      <c r="J20" s="5">
+        <f t="shared" si="7"/>
+        <v>249</v>
+      </c>
+      <c r="K20" s="5">
+        <f t="shared" si="7"/>
+        <v>173</v>
+      </c>
+      <c r="L20" s="5">
+        <f t="shared" si="7"/>
+        <v>172</v>
+      </c>
+      <c r="M20" s="5">
+        <f t="shared" si="7"/>
+        <v>115</v>
+      </c>
+      <c r="N20" s="5">
+        <f t="shared" si="8"/>
+        <v>44</v>
+      </c>
       <c r="O20" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="O20:O31" si="10">O19+O4</f>
         <v>36</v>
       </c>
       <c r="Q20" s="2">
@@ -1352,228 +1554,695 @@
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <f t="shared" si="7"/>
+        <v>516</v>
+      </c>
+      <c r="B21" s="5">
+        <f t="shared" si="7"/>
+        <v>492</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" si="7"/>
+        <v>501</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="7"/>
+        <v>492</v>
+      </c>
+      <c r="E21" s="5">
+        <f t="shared" si="7"/>
+        <v>504</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" si="7"/>
+        <v>460</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="7"/>
+        <v>351</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="7"/>
+        <v>298</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" si="7"/>
+        <v>225</v>
+      </c>
+      <c r="J21" s="5">
+        <f t="shared" si="7"/>
+        <v>255</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" si="7"/>
+        <v>201</v>
+      </c>
+      <c r="L21" s="5">
+        <f t="shared" si="7"/>
+        <v>195</v>
+      </c>
+      <c r="M21" s="5">
+        <f t="shared" si="7"/>
+        <v>129</v>
+      </c>
+      <c r="N21" s="5">
+        <f t="shared" si="8"/>
+        <v>103</v>
+      </c>
       <c r="O21" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <f t="shared" si="7"/>
+        <v>544</v>
+      </c>
+      <c r="B22" s="5">
+        <f t="shared" si="7"/>
+        <v>574</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" si="7"/>
+        <v>552</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="7"/>
+        <v>532</v>
+      </c>
+      <c r="E22" s="5">
+        <f t="shared" si="7"/>
+        <v>502</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" si="7"/>
+        <v>490</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" si="7"/>
+        <v>363</v>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" si="7"/>
+        <v>346</v>
+      </c>
+      <c r="I22" s="5">
+        <f t="shared" si="7"/>
+        <v>309</v>
+      </c>
+      <c r="J22" s="5">
+        <f t="shared" si="7"/>
+        <v>271</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" si="7"/>
+        <v>222</v>
+      </c>
+      <c r="L22" s="5">
+        <f t="shared" si="7"/>
+        <v>226</v>
+      </c>
+      <c r="M22" s="5">
+        <f t="shared" si="7"/>
+        <v>157</v>
+      </c>
+      <c r="N22" s="5">
+        <f t="shared" si="8"/>
+        <v>79</v>
+      </c>
       <c r="O22" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <f t="shared" si="7"/>
+        <v>541</v>
+      </c>
+      <c r="B23" s="5">
+        <f t="shared" si="7"/>
+        <v>537</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" si="7"/>
+        <v>577</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="7"/>
+        <v>515</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" si="7"/>
+        <v>492</v>
+      </c>
+      <c r="F23" s="5">
+        <f t="shared" si="7"/>
+        <v>451</v>
+      </c>
+      <c r="G23" s="5">
+        <f t="shared" si="7"/>
+        <v>389</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" si="7"/>
+        <v>341</v>
+      </c>
+      <c r="I23" s="5">
+        <f t="shared" si="7"/>
+        <v>292</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" si="7"/>
+        <v>300</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="7"/>
+        <v>243</v>
+      </c>
+      <c r="L23" s="5">
+        <f t="shared" si="7"/>
+        <v>238</v>
+      </c>
+      <c r="M23" s="5">
+        <f t="shared" si="7"/>
+        <v>128</v>
+      </c>
+      <c r="N23" s="5">
+        <f t="shared" si="8"/>
+        <v>64</v>
+      </c>
       <c r="O23" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <f t="shared" si="7"/>
+        <v>668</v>
+      </c>
+      <c r="B24" s="5">
+        <f t="shared" si="7"/>
+        <v>654</v>
+      </c>
+      <c r="C24" s="5">
+        <f t="shared" si="7"/>
+        <v>629</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="7"/>
+        <v>508</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="7"/>
+        <v>488</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" si="7"/>
+        <v>493</v>
+      </c>
+      <c r="G24" s="5">
+        <f t="shared" si="7"/>
+        <v>400</v>
+      </c>
+      <c r="H24" s="5">
+        <f t="shared" si="7"/>
+        <v>383</v>
+      </c>
+      <c r="I24" s="5">
+        <f t="shared" si="7"/>
+        <v>387</v>
+      </c>
+      <c r="J24" s="5">
+        <f t="shared" si="7"/>
+        <v>331</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="7"/>
+        <v>275</v>
+      </c>
+      <c r="L24" s="5">
+        <f t="shared" si="7"/>
+        <v>229</v>
+      </c>
+      <c r="M24" s="5">
+        <f t="shared" si="7"/>
+        <v>186</v>
+      </c>
+      <c r="N24" s="5">
+        <f t="shared" si="8"/>
+        <v>49</v>
+      </c>
       <c r="O24" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <f t="shared" si="7"/>
+        <v>712</v>
+      </c>
+      <c r="B25" s="5">
+        <f t="shared" si="7"/>
+        <v>639</v>
+      </c>
+      <c r="C25" s="5">
+        <f t="shared" si="7"/>
+        <v>626</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="7"/>
+        <v>584</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="7"/>
+        <v>529</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="7"/>
+        <v>513</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" si="7"/>
+        <v>514</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" si="7"/>
+        <v>462</v>
+      </c>
+      <c r="I25" s="5">
+        <f t="shared" si="7"/>
+        <v>433</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" si="7"/>
+        <v>350</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="7"/>
+        <v>330</v>
+      </c>
+      <c r="L25" s="5">
+        <f t="shared" si="7"/>
+        <v>278</v>
+      </c>
+      <c r="M25" s="5">
+        <f t="shared" si="7"/>
+        <v>164</v>
+      </c>
+      <c r="N25" s="5">
+        <f t="shared" si="8"/>
+        <v>112</v>
+      </c>
       <c r="O25" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <f t="shared" si="7"/>
+        <v>746</v>
+      </c>
+      <c r="B26" s="5">
+        <f t="shared" si="7"/>
+        <v>675</v>
+      </c>
+      <c r="C26" s="5">
+        <f t="shared" si="7"/>
+        <v>637</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="7"/>
+        <v>615</v>
+      </c>
+      <c r="E26" s="5">
+        <f t="shared" si="7"/>
+        <v>600</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" si="7"/>
+        <v>540</v>
+      </c>
+      <c r="G26" s="5">
+        <f t="shared" si="7"/>
+        <v>543</v>
+      </c>
+      <c r="H26" s="5">
+        <f t="shared" si="7"/>
+        <v>503</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" si="7"/>
+        <v>394</v>
+      </c>
+      <c r="J26" s="5">
+        <f t="shared" si="7"/>
+        <v>369</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" si="7"/>
+        <v>348</v>
+      </c>
+      <c r="L26" s="5">
+        <f t="shared" si="7"/>
+        <v>334</v>
+      </c>
+      <c r="M26" s="5">
+        <f t="shared" si="7"/>
+        <v>131</v>
+      </c>
+      <c r="N26" s="5">
+        <f t="shared" si="8"/>
+        <v>103</v>
+      </c>
       <c r="O26" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <f t="shared" si="7"/>
+        <v>715</v>
+      </c>
+      <c r="B27" s="5">
+        <f t="shared" si="7"/>
+        <v>665</v>
+      </c>
+      <c r="C27" s="5">
+        <f t="shared" si="7"/>
+        <v>618</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" si="7"/>
+        <v>576</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="7"/>
+        <v>568</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" si="7"/>
+        <v>576</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="7"/>
+        <v>523</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" si="7"/>
+        <v>491</v>
+      </c>
+      <c r="I27" s="5">
+        <f t="shared" si="7"/>
+        <v>456</v>
+      </c>
+      <c r="J27" s="5">
+        <f t="shared" si="7"/>
+        <v>432</v>
+      </c>
+      <c r="K27" s="5">
+        <f t="shared" si="7"/>
+        <v>403</v>
+      </c>
+      <c r="L27" s="5">
+        <f t="shared" si="7"/>
+        <v>385</v>
+      </c>
+      <c r="M27" s="5">
+        <f t="shared" si="7"/>
+        <v>123</v>
+      </c>
+      <c r="N27" s="5">
+        <f t="shared" si="8"/>
+        <v>152</v>
+      </c>
       <c r="O27" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <f t="shared" si="7"/>
+        <v>768</v>
+      </c>
+      <c r="B28" s="5">
+        <f t="shared" si="7"/>
+        <v>695</v>
+      </c>
+      <c r="C28" s="5">
+        <f t="shared" si="7"/>
+        <v>618</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" si="7"/>
+        <v>591</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="7"/>
+        <v>567</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" si="7"/>
+        <v>537</v>
+      </c>
+      <c r="G28" s="5">
+        <f t="shared" si="7"/>
+        <v>489</v>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" si="7"/>
+        <v>468</v>
+      </c>
+      <c r="I28" s="5">
+        <f t="shared" si="7"/>
+        <v>491</v>
+      </c>
+      <c r="J28" s="5">
+        <f t="shared" si="7"/>
+        <v>408</v>
+      </c>
+      <c r="K28" s="5">
+        <f t="shared" si="7"/>
+        <v>408</v>
+      </c>
+      <c r="L28" s="5">
+        <f t="shared" si="7"/>
+        <v>383</v>
+      </c>
+      <c r="M28" s="5">
+        <f t="shared" si="7"/>
+        <v>174</v>
+      </c>
+      <c r="N28" s="5">
+        <f t="shared" si="8"/>
+        <v>146</v>
+      </c>
       <c r="O28" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <f t="shared" si="7"/>
+        <v>740</v>
+      </c>
+      <c r="B29" s="5">
+        <f t="shared" si="7"/>
+        <v>664</v>
+      </c>
+      <c r="C29" s="5">
+        <f t="shared" si="7"/>
+        <v>644</v>
+      </c>
+      <c r="D29" s="5">
+        <f t="shared" si="7"/>
+        <v>564</v>
+      </c>
+      <c r="E29" s="5">
+        <f t="shared" si="7"/>
+        <v>593</v>
+      </c>
+      <c r="F29" s="5">
+        <f t="shared" si="7"/>
+        <v>506</v>
+      </c>
+      <c r="G29" s="5">
+        <f t="shared" si="7"/>
+        <v>498</v>
+      </c>
+      <c r="H29" s="5">
+        <f t="shared" si="7"/>
+        <v>455</v>
+      </c>
+      <c r="I29" s="5">
+        <f t="shared" si="7"/>
+        <v>483</v>
+      </c>
+      <c r="J29" s="5">
+        <f t="shared" si="7"/>
+        <v>423</v>
+      </c>
+      <c r="K29" s="5">
+        <f t="shared" si="7"/>
+        <v>396</v>
+      </c>
+      <c r="L29" s="5">
+        <f t="shared" si="7"/>
+        <v>396</v>
+      </c>
+      <c r="M29" s="5">
+        <f t="shared" si="7"/>
+        <v>189</v>
+      </c>
+      <c r="N29" s="5">
+        <f t="shared" si="8"/>
+        <v>146</v>
+      </c>
       <c r="O29" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>124</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <f t="shared" si="7"/>
+        <v>786</v>
+      </c>
+      <c r="B30" s="5">
+        <f t="shared" si="7"/>
+        <v>685</v>
+      </c>
+      <c r="C30" s="5">
+        <f t="shared" si="7"/>
+        <v>620</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" si="7"/>
+        <v>634</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" si="7"/>
+        <v>627</v>
+      </c>
+      <c r="F30" s="5">
+        <f t="shared" si="7"/>
+        <v>466</v>
+      </c>
+      <c r="G30" s="5">
+        <f t="shared" si="7"/>
+        <v>492</v>
+      </c>
+      <c r="H30" s="5">
+        <f t="shared" si="7"/>
+        <v>499</v>
+      </c>
+      <c r="I30" s="5">
+        <f t="shared" si="7"/>
+        <v>505</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" si="7"/>
+        <v>484</v>
+      </c>
+      <c r="K30" s="5">
+        <f t="shared" si="7"/>
+        <v>430</v>
+      </c>
+      <c r="L30" s="5">
+        <f t="shared" si="7"/>
+        <v>410</v>
+      </c>
+      <c r="M30" s="5">
+        <f t="shared" si="7"/>
+        <v>156</v>
+      </c>
+      <c r="N30" s="5">
+        <f t="shared" si="8"/>
+        <v>148</v>
+      </c>
       <c r="O30" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>157</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <f t="shared" ref="A31:M31" si="11">MAX(A30,B30,B31)+A15</f>
+        <v>842</v>
+      </c>
+      <c r="B31" s="5">
+        <f t="shared" si="11"/>
+        <v>785</v>
+      </c>
+      <c r="C31" s="5">
+        <f t="shared" si="11"/>
+        <v>756</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" si="11"/>
+        <v>701</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" si="11"/>
+        <v>661</v>
+      </c>
+      <c r="F31" s="5">
+        <f t="shared" si="11"/>
+        <v>475</v>
+      </c>
+      <c r="G31" s="5">
+        <f t="shared" si="11"/>
+        <v>508</v>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" si="11"/>
+        <v>522</v>
+      </c>
+      <c r="I31" s="5">
+        <f t="shared" si="11"/>
+        <v>527</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" si="11"/>
+        <v>525</v>
+      </c>
+      <c r="K31" s="5">
+        <f t="shared" si="11"/>
+        <v>469</v>
+      </c>
+      <c r="L31" s="5">
+        <f t="shared" si="11"/>
+        <v>374</v>
+      </c>
+      <c r="M31" s="5">
+        <f t="shared" si="11"/>
+        <v>191</v>
+      </c>
+      <c r="N31" s="5">
+        <f>MAX(N30,O30,O31)+N15</f>
+        <v>185</v>
+      </c>
       <c r="O31" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="10"/>
         <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>